<commit_message>
Updated summary UNITED tables
</commit_message>
<xml_diff>
--- a/Supplementary_Material/Outputs/UNITED_T1D_table.xlsx
+++ b/Supplementary_Material/Outputs/UNITED_T1D_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -881,6 +881,33 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>durationfinal</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14.23 [5.82,23.53]</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0 (0%)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>14.4 [13.66,18.1]</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0 (0%)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>